<commit_message>
Agrego Medico Auditor en el reporte Debitos
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Efectores/parametros_servidor.xlsx
+++ b/DBA/Reportes BI/2021/Efectores/parametros_servidor.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personales\Sistemas\Agustin\Reportes BI\2021\Efectores\version2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Efectores\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Parametros servidor</t>
   </si>
@@ -65,22 +65,19 @@
     <t>facoep2017</t>
   </si>
   <si>
-    <t>openpg</t>
-  </si>
-  <si>
-    <t>openpgpwd</t>
-  </si>
-  <si>
     <t>C:/Users/User/Desktop/FACOEP/DBA/Reportes BI/2021/Efectores</t>
   </si>
   <si>
     <t>E:/Personales/Sistemas/Agustin/Reportes BI/2021/Efectores/version2</t>
+  </si>
+  <si>
+    <t>odoo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,7 +404,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +432,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -443,10 +440,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -454,10 +451,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -465,10 +462,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -479,7 +476,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -490,7 +487,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,7 +498,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -509,10 +506,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>